<commit_message>
Update DSM CXO Dashboards Plan.xlsx
</commit_message>
<xml_diff>
--- a/1 eCommerce/presentations/DSM CXO Dashboards Plan.xlsx
+++ b/1 eCommerce/presentations/DSM CXO Dashboards Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/063bf5775d666102/__DSM_LMS_Courses_New/LEVEL 1 - Data Transition Specialist/CXO_Dashboards/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\DSM GITHUB\DSM_CXO_Executive_Dashboards\1 eCommerce\presentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="274" documentId="8_{6882FE3C-B940-4613-83A3-2A1147570650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C289E45F-9D56-457B-A425-205559FF49E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182AC4C8-2CCA-467C-9F15-02DEE2B5D788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="724" xr2:uid="{8136B31D-7A3F-4920-AE42-32CA5D616737}"/>
   </bookViews>
@@ -26,6 +26,7 @@
     <sheet name="CPO_HR" sheetId="21" r:id="rId11"/>
     <sheet name="CSO_Sustainability" sheetId="22" r:id="rId12"/>
     <sheet name="CDO" sheetId="23" r:id="rId13"/>
+    <sheet name="links" sheetId="24" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="128">
   <si>
     <t>Role</t>
   </si>
@@ -464,6 +465,12 @@
   </si>
   <si>
     <t>CxO Roles and Objectives (openai.com)</t>
+  </si>
+  <si>
+    <t>ChatGPT (openai.com)</t>
+  </si>
+  <si>
+    <t>CEO Explanation</t>
   </si>
 </sst>
 </file>
@@ -472,9 +479,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -568,7 +575,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -585,9 +592,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -597,25 +601,25 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -642,7 +646,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -662,7 +665,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -682,10 +684,51 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -725,8 +768,33 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -745,10 +813,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.0%"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="164" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -768,6 +833,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -787,7 +853,33 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -806,6 +898,47 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -845,15 +978,12 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="none"/>
+        <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -872,7 +1002,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -892,8 +1021,32 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -912,7 +1065,45 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -957,10 +1148,28 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -998,6 +1207,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1017,7 +1250,72 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1037,8 +1335,10 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1057,6 +1357,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1139,7 +1440,66 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1184,6 +1544,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1203,7 +1564,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1223,33 +1584,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1268,7 +1604,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1288,7 +1623,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1308,33 +1642,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1353,7 +1661,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1376,322 +1686,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1756,78 +1760,78 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A3D2B3D5-F7D7-4025-A47A-2C3AFB504A4E}" name="Table3567891011" displayName="Table3567891011" ref="A1:D11" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" dataCellStyle="Comma">
   <autoFilter ref="A1:D11" xr:uid="{583BCF46-B88C-49C9-8A9A-2BDBA1B92663}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{97C9AB2F-F513-45D8-958D-812FB97E0C0B}" name="Quarter" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{1D394DD5-32A4-4C48-9DDE-6F3430C4B202}" name="NPS" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{46F27784-6033-4565-A0A2-6136669B34DD}" name="CSAT (%)" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{D4E05732-8EA2-4C41-9053-51974D3AAC3A}" name="Customer Support Response Time (hours)" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{97C9AB2F-F513-45D8-958D-812FB97E0C0B}" name="Quarter" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{1D394DD5-32A4-4C48-9DDE-6F3430C4B202}" name="NPS" dataDxfId="20" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{46F27784-6033-4565-A0A2-6136669B34DD}" name="CSAT (%)" dataDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{D4E05732-8EA2-4C41-9053-51974D3AAC3A}" name="Customer Support Response Time (hours)" dataDxfId="18" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A9C28E6A-7CE0-4F18-93EA-E1E8C5DD5FD2}" name="Table356789101112" displayName="Table356789101112" ref="A1:D11" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A9C28E6A-7CE0-4F18-93EA-E1E8C5DD5FD2}" name="Table356789101112" displayName="Table356789101112" ref="A1:D11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" dataCellStyle="Comma">
   <autoFilter ref="A1:D11" xr:uid="{583BCF46-B88C-49C9-8A9A-2BDBA1B92663}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{46C7A00E-AF84-4310-B2EE-CE08713BD804}" name="Quarter" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{CD69291B-7779-427F-BE8C-EBC004089AEB}" name="Employee Turnover Rate (%)" dataDxfId="18" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{2845B2A8-4AAF-4D36-AC77-E3EB09BC1899}" name="Time to Fill Positions (days)" dataDxfId="17" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{8ECF8E39-0DD9-4380-8CFC-5F9FF6A8033E}" name="Employee Satisfaction Index" dataDxfId="16" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{46C7A00E-AF84-4310-B2EE-CE08713BD804}" name="Quarter" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{CD69291B-7779-427F-BE8C-EBC004089AEB}" name="Employee Turnover Rate (%)" dataDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{2845B2A8-4AAF-4D36-AC77-E3EB09BC1899}" name="Time to Fill Positions (days)" dataDxfId="13" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{8ECF8E39-0DD9-4380-8CFC-5F9FF6A8033E}" name="Employee Satisfaction Index" dataDxfId="12" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{39BA2565-FFAF-4D05-B3CF-0BE8C3C896EC}" name="Table35678910111213" displayName="Table35678910111213" ref="A1:D11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{39BA2565-FFAF-4D05-B3CF-0BE8C3C896EC}" name="Table35678910111213" displayName="Table35678910111213" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" dataCellStyle="Comma">
   <autoFilter ref="A1:D11" xr:uid="{583BCF46-B88C-49C9-8A9A-2BDBA1B92663}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8F67744D-5FC0-47B7-8737-54F9A7F30AF8}" name="Quarter" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{D14AFD77-F727-4025-B500-D4D5121CE273}" name="Carbon Footprint Reduction (%)" dataDxfId="6" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{CFD05E39-EFD0-4FB6-88C0-E3C927291413}" name="Percentage of Sustainable Materials Used (%)" dataDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{586C4244-F093-4136-A88C-58106977B42B}" name="Sustainability Index Score" dataDxfId="5" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{8F67744D-5FC0-47B7-8737-54F9A7F30AF8}" name="Quarter" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{D14AFD77-F727-4025-B500-D4D5121CE273}" name="Carbon Footprint Reduction (%)" dataDxfId="8" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{CFD05E39-EFD0-4FB6-88C0-E3C927291413}" name="Percentage of Sustainable Materials Used (%)" dataDxfId="7" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{586C4244-F093-4136-A88C-58106977B42B}" name="Sustainability Index Score" dataDxfId="6" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{12904B1E-4C90-4997-B333-1AAA0953E474}" name="Table3567891011121314" displayName="Table3567891011121314" ref="A1:D11" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{12904B1E-4C90-4997-B333-1AAA0953E474}" name="Table3567891011121314" displayName="Table3567891011121314" ref="A1:D11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" dataCellStyle="Comma">
   <autoFilter ref="A1:D11" xr:uid="{583BCF46-B88C-49C9-8A9A-2BDBA1B92663}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E2EE2ABC-1351-4468-920C-0781588A2BD4}" name="Quarter" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{4A8FC451-13B0-400C-B72F-0172C26BA295}" name="Accuracy of Sales Forecasts (%)" dataDxfId="10" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{7726F5C0-BB99-457D-B237-E14319334D33}" name="Data Quality Score" dataDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{451DC817-C989-4A9A-8897-23E7780F3007}" name="Compliance Rate with Data Protection Laws (%)" dataDxfId="8" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{E2EE2ABC-1351-4468-920C-0781588A2BD4}" name="Quarter" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{4A8FC451-13B0-400C-B72F-0172C26BA295}" name="Accuracy of Sales Forecasts (%)" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{7726F5C0-BB99-457D-B237-E14319334D33}" name="Data Quality Score" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{451DC817-C989-4A9A-8897-23E7780F3007}" name="Compliance Rate with Data Protection Laws (%)" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B6B5B191-CC01-419F-9B9A-C100CF83CFA1}" name="Table2" displayName="Table2" ref="A2:C8" totalsRowShown="0" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B6B5B191-CC01-419F-9B9A-C100CF83CFA1}" name="Table2" displayName="Table2" ref="A2:C8" totalsRowShown="0" dataDxfId="76">
   <autoFilter ref="A2:C8" xr:uid="{B6B5B191-CC01-419F-9B9A-C100CF83CFA1}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4BADA143-9AA4-49D2-A766-2E64CF712D97}" name="Aspect" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{05FA3FBE-C846-4159-9373-C216421C2590}" name="OKR (Objectives and Key Results)" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{9F35851A-0E84-4D14-924A-D0C830DB6BBF}" name="KPI (Key Performance Indicators)" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{4BADA143-9AA4-49D2-A766-2E64CF712D97}" name="Aspect" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{05FA3FBE-C846-4159-9373-C216421C2590}" name="OKR (Objectives and Key Results)" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{9F35851A-0E84-4D14-924A-D0C830DB6BBF}" name="KPI (Key Performance Indicators)" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{583BCF46-B88C-49C9-8A9A-2BDBA1B92663}" name="Table3" displayName="Table3" ref="A1:H11" totalsRowShown="0" headerRowDxfId="63" dataDxfId="64" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{583BCF46-B88C-49C9-8A9A-2BDBA1B92663}" name="Table3" displayName="Table3" ref="A1:H11" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" dataCellStyle="Comma">
   <autoFilter ref="A1:H11" xr:uid="{583BCF46-B88C-49C9-8A9A-2BDBA1B92663}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{49FC9FBE-D37D-4F9E-87C5-D9460394B221}" name="Quarter" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{8EDF6DA4-3B43-400C-ADCC-DEA8598D79EF}" name="Overall Revenue Growth" dataDxfId="71" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{E7E539A3-B261-432B-A6BE-EA52894FC9DE}" name="Market Share" dataDxfId="70" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{34FFD8D4-D1A3-4FB8-B1AF-3B23E066DAC4}" name="Employee Engagement Score" dataDxfId="69" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{0CBE50C8-8C17-4876-B595-8378DEA2BE3A}" name="Customer Satisfaction Score" dataDxfId="68" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{C5A3EA2F-F1A7-4D34-9F83-42A45403BDB2}" name="Revenue" dataDxfId="67" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{1E5B0366-11E0-4389-A82E-130C9695C549}" name="Cost" dataDxfId="66" dataCellStyle="Comma"/>
-    <tableColumn id="8" xr3:uid="{E8974942-CDDF-423D-81B1-E7759ED3CB06}" name="Profit" dataDxfId="65" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{49FC9FBE-D37D-4F9E-87C5-D9460394B221}" name="Quarter" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{8EDF6DA4-3B43-400C-ADCC-DEA8598D79EF}" name="Overall Revenue Growth" dataDxfId="69" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{E7E539A3-B261-432B-A6BE-EA52894FC9DE}" name="Market Share" dataDxfId="68" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{34FFD8D4-D1A3-4FB8-B1AF-3B23E066DAC4}" name="Employee Engagement Score" dataDxfId="67" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{0CBE50C8-8C17-4876-B595-8378DEA2BE3A}" name="Customer Satisfaction Score" dataDxfId="66" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{C5A3EA2F-F1A7-4D34-9F83-42A45403BDB2}" name="Revenue" dataDxfId="65" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{1E5B0366-11E0-4389-A82E-130C9695C549}" name="Cost" dataDxfId="64" dataCellStyle="Comma"/>
+    <tableColumn id="8" xr3:uid="{E8974942-CDDF-423D-81B1-E7759ED3CB06}" name="Profit" dataDxfId="63" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1840,8 +1844,8 @@
     <tableColumn id="1" xr3:uid="{4F503721-2868-4565-AF0D-9CBAF32EC80E}" name="Quarter" dataDxfId="60"/>
     <tableColumn id="2" xr3:uid="{F7ED1AB2-4753-49AA-94FF-696548536371}" name="Order Fulfillment Time (days)" dataDxfId="59" dataCellStyle="Comma"/>
     <tableColumn id="3" xr3:uid="{EB456C65-A0BF-476B-9403-699152EB6C41}" name="COGS (in thousands)" dataDxfId="58" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{09FAF87F-5242-4532-90EE-01A3EC162C32}" name="Inventory Turnover Rate" dataDxfId="56" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{C6347ECB-4807-4B4A-BEB6-71EB81B498DF}" name="On-time Delivery Rate (%)" dataDxfId="57" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{09FAF87F-5242-4532-90EE-01A3EC162C32}" name="Inventory Turnover Rate" dataDxfId="57" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{C6347ECB-4807-4B4A-BEB6-71EB81B498DF}" name="On-time Delivery Rate (%)" dataDxfId="56" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1881,34 +1885,34 @@
     <tableColumn id="2" xr3:uid="{B62172BE-52D9-4500-9D55-05C2A1844013}" name="App Downloads" dataDxfId="40" dataCellStyle="Comma"/>
     <tableColumn id="3" xr3:uid="{0C57DAD5-80AB-4DBB-B3D6-06A5F9EA96F9}" name="Active Users" dataDxfId="39" dataCellStyle="Comma"/>
     <tableColumn id="4" xr3:uid="{507CC722-0E9F-449F-8B9A-B0BD47E4AE94}" name="Website Uptime (%)" dataDxfId="38" dataCellStyle="Percent"/>
-    <tableColumn id="10" xr3:uid="{6680CF64-CEC9-4E31-BC21-F4246D989F6B}" name="Website Speed (sec)" dataDxfId="27" dataCellStyle="Comma"/>
-    <tableColumn id="11" xr3:uid="{13D6BA88-8E7E-4611-B1D1-28DA85BF6AC1}" name="Tech Stack ROI" dataDxfId="26" dataCellStyle="Comma"/>
+    <tableColumn id="10" xr3:uid="{6680CF64-CEC9-4E31-BC21-F4246D989F6B}" name="Website Speed (sec)" dataDxfId="37" dataCellStyle="Comma"/>
+    <tableColumn id="11" xr3:uid="{13D6BA88-8E7E-4611-B1D1-28DA85BF6AC1}" name="Tech Stack ROI" dataDxfId="36" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C3F44148-76EC-49CB-B5C3-178079E84D1B}" name="Table356789" displayName="Table356789" ref="A1:D11" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C3F44148-76EC-49CB-B5C3-178079E84D1B}" name="Table356789" displayName="Table356789" ref="A1:D11" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" dataCellStyle="Comma">
   <autoFilter ref="A1:D11" xr:uid="{583BCF46-B88C-49C9-8A9A-2BDBA1B92663}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{56E5ADFC-318B-486D-BADC-323895ED9B4C}" name="Quarter" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{9FEC52A4-CDF8-4599-80B5-F0D1952D363B}" name="Sales Growth Rate (%)" dataDxfId="25" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{7C3C4290-4741-45C8-BFFB-DB78799E8146}" name="Market Penetration Rate (%)" dataDxfId="24" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{C6CD45A1-B377-4627-881C-A7EE319A2F39}" name="CLTV (in units)" dataDxfId="34" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{56E5ADFC-318B-486D-BADC-323895ED9B4C}" name="Quarter" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{9FEC52A4-CDF8-4599-80B5-F0D1952D363B}" name="Sales Growth Rate (%)" dataDxfId="32" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{7C3C4290-4741-45C8-BFFB-DB78799E8146}" name="Market Penetration Rate (%)" dataDxfId="31" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{C6CD45A1-B377-4627-881C-A7EE319A2F39}" name="CLTV (in units)" dataDxfId="30" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2DCA2ABE-79F3-47D3-A763-51B2D4954B2B}" name="Table35678910" displayName="Table35678910" ref="A1:D11" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2DCA2ABE-79F3-47D3-A763-51B2D4954B2B}" name="Table35678910" displayName="Table35678910" ref="A1:D11" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" dataCellStyle="Comma">
   <autoFilter ref="A1:D11" xr:uid="{583BCF46-B88C-49C9-8A9A-2BDBA1B92663}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{096A844C-BE6C-41AF-BCEC-53BF528803E1}" name="Quarter" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{78BA2881-6721-4E57-8CF0-AD15D4608290}" name="Product Development Cycle Time (months)" dataDxfId="30" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{44FAE8BB-70E6-4407-BBE8-08A18E17C979}" name="Gross Margin per Product Line (%)" dataDxfId="29" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{0458049F-C1A7-406E-9772-F8E738718616}" name="Product Return Rate (%)" dataDxfId="28" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{096A844C-BE6C-41AF-BCEC-53BF528803E1}" name="Quarter" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{78BA2881-6721-4E57-8CF0-AD15D4608290}" name="Product Development Cycle Time (months)" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{44FAE8BB-70E6-4407-BBE8-08A18E17C979}" name="Gross Margin per Product Line (%)" dataDxfId="25" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{0458049F-C1A7-406E-9772-F8E738718616}" name="Product Return Rate (%)" dataDxfId="24" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2165,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB94902B-9358-449C-9790-539750B79010}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,13 +2185,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2391,35 +2395,15 @@
       </c>
       <c r="E13" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="16" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B28" r:id="rId1" display="https://chat.openai.com/c/caf6e3e1-1069-486f-a035-d12c9e4d08a1" xr:uid="{831BC3EE-8A6F-410F-ADD9-4911588435A3}"/>
-    <hyperlink ref="B29" r:id="rId2" display="https://chat.openai.com/c/8eb511d8-b0f2-41fa-8d35-d6d0ab090c72" xr:uid="{4AB6BD97-CD94-4F19-A954-B48F50092215}"/>
-    <hyperlink ref="B30" r:id="rId3" display="https://chat.openai.com/c/a3f0f061-b3cc-48e1-a141-4656a2a38a3f" xr:uid="{3CAF07FE-4326-43A0-891C-F095E24B77C9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2439,219 +2423,219 @@
     <col min="4" max="4" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>0.7</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <v>0.8</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <v>0.04</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>0.72</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>0.81</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>0.74</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>0.82</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>0.76</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <v>0.83</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>3.2500000000000001E-2</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>0.78</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>0.84</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>0.03</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>0.8</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>0.85</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>2.75E-2</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>0.82</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>0.86</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>0.84</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <v>0.87</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>0.86</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>0.88</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>0.02</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>0.88</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <v>0.89</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2676,219 +2660,219 @@
     <col min="4" max="4" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>10</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>45</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>70</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>9</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>43</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>72</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>8</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>41</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>74</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>7</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>39</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>76</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>6</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>37</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>78</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>5</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>35</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>80</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>33</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>82</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>5</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>31</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>84</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>5</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>30</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>86</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>5</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>30</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>88</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2913,223 +2897,223 @@
     <col min="4" max="4" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>0</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="8">
         <v>0.5</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>50</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>0</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="8">
         <v>0.5</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>55</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>0</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="8">
         <v>0.5</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>60</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>0</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="8">
         <v>0.5</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>65</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="8">
         <v>0.6</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>70</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="8">
         <v>0.6</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>75</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="8">
         <v>0.6</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>80</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="8">
         <v>0.6</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>85</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>0.05</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="8">
         <v>0.7</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>90</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>0.05</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="8">
         <v>0.7</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>95</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3154,233 +3138,281 @@
     <col min="4" max="4" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>0.7</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>0.75</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0.9</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>0.72</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>0.77500000000000002</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>0.91</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>0.74</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>0.8</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>0.92</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>0.76</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>0.82499999999999996</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>0.93</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.78</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>0.85</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.94</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>0.8</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>0.875</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>0.95</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>0.82</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>0.9</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>0.96</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>0.84</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>0.92500000000000004</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>0.97</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>0.86</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>0.95</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>0.98</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>0.88</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>0.97499999999999998</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>0.99</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A312911-5189-4841-9852-6ADDD239E6E7}">
+  <dimension ref="B2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://chat.openai.com/c/caf6e3e1-1069-486f-a035-d12c9e4d08a1" xr:uid="{831BC3EE-8A6F-410F-ADD9-4911588435A3}"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://chat.openai.com/c/8eb511d8-b0f2-41fa-8d35-d6d0ab090c72" xr:uid="{4AB6BD97-CD94-4F19-A954-B48F50092215}"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://chat.openai.com/c/a3f0f061-b3cc-48e1-a141-4656a2a38a3f" xr:uid="{3CAF07FE-4326-43A0-891C-F095E24B77C9}"/>
+    <hyperlink ref="C5" r:id="rId4" display="https://chat.openai.com/c/38749779-b331-4209-94a2-6f9a6bc45400" xr:uid="{AF4D0822-CD9E-45CF-B5F5-483727BEA908}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3399,11 +3431,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3509,319 +3541,319 @@
     <col min="6" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>0.05</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>0.15</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0.7</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>0.85</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <v>105000</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>70000</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <v>35000</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>0.16</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>0.72</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>0.87</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>112350</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <v>73500</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <v>38850</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>0.06</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>0.17</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>0.74</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>0.89</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>119091</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>77000</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>42091</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>0.08</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>0.18</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>0.76</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>0.9</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>128618</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>80500</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <v>48118</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.1</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>0.19</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.78</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>0.91</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <v>141480</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <v>84000</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <v>57480</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>0.09</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>0.2</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>0.8</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>0.92</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>154213</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>87500</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>66713</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>0.11</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>0.21</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>0.82</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>0.93</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>171177</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>91000</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>80177</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>0.12</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>0.22</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>0.84</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>0.94</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>191718</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <v>94500</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>97218</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>0.13</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>0.23</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>0.86</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>0.95</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>216641</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <v>98000</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>118641</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>0.24</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>0.88</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>0.96</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>246971</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <v>101500</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>145471</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3847,208 +3879,208 @@
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <v>10</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>70000</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>4</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>0.9</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>68600</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>4.08</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>0.9</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>9.6</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>67200</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>4.16</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>0.9</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>9.4</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>65800</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>4.24</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>0.9</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>64400.000000000007</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>4.32</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>0.9</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>9</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>63000</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>0.95</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>8.8000000000000007</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>61600</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>4.4800000000000004</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>0.95</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>8.6</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>60200</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>4.5599999999999996</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>0.95</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>8.4</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>58800</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>4.6399999999999997</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>0.95</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>57400</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>4.72</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>0.95</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" s="7"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" s="7"/>
+      <c r="F13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4073,223 +4105,223 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>0.2</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>0.15</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>100</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>0.21</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>0.16</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>105</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>0.22</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>0.17</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>110</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>0.23</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>0.18</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>115</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.24</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>0.19</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>120</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>0.25</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>0.2</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>125</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>0.26</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>0.21</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>130</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>0.27</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>0.22</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>135</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>0.23</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>140</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>0.28999999999999998</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>0.24</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>145</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4314,175 +4346,175 @@
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <v>50</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>4</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>10</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>49.25</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>4.2</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>11</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>48.51</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>4.41</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>12.1</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>47.78</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>4.63</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>13.31</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>47.07</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>4.8600000000000003</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>14.64</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>46.36</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>5.1100000000000003</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>16.11</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>45.67</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>5.36</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>17.72</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>44.98</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>5.63</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>19.489999999999998</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>44.31</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>5.91</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>21.44</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>43.64</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>6.21</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>23.58</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4509,253 +4541,253 @@
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <v>10000</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>5000</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0.99</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>2</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="12">
         <v>2</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>12000</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>6250</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>0.99099999999999999</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>1.9</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="12">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>14000</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>7500</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>0.99199999999999999</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>1.8</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <v>2.6</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>16000</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>8750</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>0.99299999999999999</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>1.7</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <v>2.9</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>18000</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>10000</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.99400000000000011</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>1.6</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <v>3.2</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>20000</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>11250</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>0.995</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>1.5</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>3.5</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>22000</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>12500</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>0.996</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>1.4</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>3.8</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>24000</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>13750</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>0.997</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>1.3</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>26000</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>15000</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>0.998</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>1.2</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>28000</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>16250</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>0.99900000000000011</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <v>4.7</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4780,197 +4812,197 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>0.2</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>0.1</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>500</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>0.2</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>0.12</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>515</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>0.2</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>530</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>0.2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>0.16</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>545</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.25</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>0.18</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>560</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>0.25</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>0.2</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>575</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>0.25</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>0.22</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>590</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>0.25</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>0.24</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>605</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>0.3</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>0.26</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>620</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>0.3</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>635</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4995,219 +5027,219 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>0.12</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>0.3</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0.05</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>0.11</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>0.3</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>0.1</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>0.3</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>0.04</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>0.09</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>0.3</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.08</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>0.3</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.03</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>0.3</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>0.06</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>0.3</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>0.02</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>0.06</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>0.3</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>0.02</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>0.06</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>0.3</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>0.02</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>0.06</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>0.3</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>0.02</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>